<commit_message>
added figures for convergence border
</commit_message>
<xml_diff>
--- a/documents/master_thesis/figures/comparison.xlsx
+++ b/documents/master_thesis/figures/comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benedikt\Entwicklung\LoadFlow\dev\documents\master_thesis\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benediktibk\Entwicklung\Loadflow\dev\documents\master_thesis\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>time 1</t>
-  </si>
-  <si>
-    <t>accuracy [W]</t>
   </si>
   <si>
     <t>time 2</t>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>HELM 200 Bit</t>
+  </si>
+  <si>
+    <t>accuracy []</t>
   </si>
 </sst>
 </file>
@@ -545,11 +545,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="388686072"/>
-        <c:axId val="388686464"/>
+        <c:axId val="366186496"/>
+        <c:axId val="366186880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="388686072"/>
+        <c:axId val="366186496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,10 +589,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388686464"/>
+        <c:crossAx val="366186880"/>
         <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -600,7 +600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="388686464"/>
+        <c:axId val="366186880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -678,7 +678,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -710,10 +710,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388686072"/>
+        <c:crossAx val="366186496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -753,7 +753,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -783,7 +783,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1185,11 +1185,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="325478000"/>
-        <c:axId val="325483488"/>
+        <c:axId val="365561872"/>
+        <c:axId val="365562256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="325478000"/>
+        <c:axId val="365561872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,10 +1229,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325483488"/>
+        <c:crossAx val="365562256"/>
         <c:crossesAt val="1.0000000000000002E-3"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1240,7 +1240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="325483488"/>
+        <c:axId val="365562256"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1328,7 +1328,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1360,10 +1360,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325478000"/>
+        <c:crossAx val="365561872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1403,7 +1403,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1433,7 +1433,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1835,11 +1835,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="325480352"/>
-        <c:axId val="325480744"/>
+        <c:axId val="366788168"/>
+        <c:axId val="365631664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="325480352"/>
+        <c:axId val="366788168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,10 +1879,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325480744"/>
+        <c:crossAx val="365631664"/>
         <c:crossesAt val="1.0000000000000012E-22"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1890,7 +1890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="325480744"/>
+        <c:axId val="365631664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1934,7 +1934,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>relative power error [W]</a:t>
+                  <a:t>relative power error [1]</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1966,7 +1966,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1998,10 +1998,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325480352"/>
+        <c:crossAx val="366788168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -2042,7 +2042,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2072,7 +2072,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4087,8 +4087,8 @@
   <dimension ref="A1:AS8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N19" sqref="N19"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4121,7 +4121,7 @@
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -4131,7 +4131,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -4141,7 +4141,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
@@ -4151,7 +4151,7 @@
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
@@ -4161,7 +4161,7 @@
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
@@ -4176,141 +4176,141 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
       <c r="N2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s">
         <v>1</v>
       </c>
       <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>4</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>5</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>6</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>7</v>
       </c>
-      <c r="U2" t="s">
-        <v>8</v>
-      </c>
       <c r="V2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="W2" t="s">
         <v>1</v>
       </c>
       <c r="X2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>7</v>
       </c>
-      <c r="AC2" t="s">
-        <v>8</v>
-      </c>
       <c r="AD2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AE2" t="s">
         <v>1</v>
       </c>
       <c r="AF2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG2" t="s">
         <v>3</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>4</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>6</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" t="s">
-        <v>8</v>
-      </c>
       <c r="AL2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AM2" t="s">
         <v>1</v>
       </c>
       <c r="AN2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO2" t="s">
         <v>3</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>4</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>5</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>6</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>7</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4457,7 +4457,7 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4898,7 +4898,7 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>1.0000000000000001E-5</v>
@@ -5409,7 +5409,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>